<commit_message>
adds Cost to results dataset
</commit_message>
<xml_diff>
--- a/src/technology/transport-model/transport-model.xlsx
+++ b/src/technology/transport-model/transport-model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\transport-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07680DAF-09B7-45D4-9B4F-D232590C1739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2229CF1A-899D-4557-8D7D-8D80AEE0A829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1125" windowWidth="20910" windowHeight="11775" activeTab="6" xr2:uid="{7A531507-5F7F-4182-A421-E47A4FC741C9}"/>
+    <workbookView xWindow="29970" yWindow="-6090" windowWidth="12150" windowHeight="21285" firstSheet="3" activeTab="5" xr2:uid="{7A531507-5F7F-4182-A421-E47A4FC741C9}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="169">
   <si>
     <t>Technology</t>
   </si>
@@ -2397,11 +2397,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36620C0E-6B32-4F3F-9283-5A4BD286D36B}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2459,16 +2464,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2479,11 +2478,14 @@
         <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>77</v>
       </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2493,10 +2495,10 @@
         <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2507,10 +2509,10 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2521,9 +2523,23 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2536,7 +2552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA7F6E3-DC99-4262-A736-356D2AE9FB2D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
#144 updates transport model to remove scenarios
</commit_message>
<xml_diff>
--- a/src/technology/transport-model/transport-model.xlsx
+++ b/src/technology/transport-model/transport-model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\transport-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2229CF1A-899D-4557-8D7D-8D80AEE0A829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADA0BB6-303E-47B9-9F85-A0536ADF003E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="-6090" windowWidth="12150" windowHeight="21285" firstSheet="3" activeTab="5" xr2:uid="{7A531507-5F7F-4182-A421-E47A4FC741C9}"/>
+    <workbookView xWindow="30990" yWindow="345" windowWidth="17730" windowHeight="15120" tabRatio="729" activeTab="3" xr2:uid="{7A531507-5F7F-4182-A421-E47A4FC741C9}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,14 +42,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="167">
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Scenario</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
   </si>
   <si>
     <t>No Category</t>
-  </si>
-  <si>
-    <t>Business as Usual</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -902,7 +896,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C21C384-E1A6-43E8-A921-7675DB49144A}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -911,298 +907,298 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2">
         <v>100000</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
         <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
         <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
         <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
         <v>15</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
         <v>24</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <v>0.125754527</v>
       </c>
       <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
         <v>27</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11">
         <v>3.976</v>
       </c>
       <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
         <v>30</v>
-      </c>
-      <c r="G11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
         <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1223,48 +1219,48 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
-        <v>42</v>
-      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1285,183 +1281,183 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1469,13 +1465,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1483,13 +1479,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -1497,13 +1493,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1518,33 +1514,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308C4161-C0EC-416C-82DF-C9CC3CAF6B5B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1556,7 +1554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{746EF78C-EFC9-4991-94C7-3C79A5473035}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1565,36 +1565,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1603,24 +1603,24 @@
         <v>82333.333329999994</v>
       </c>
       <c r="F2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
         <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1629,24 +1629,24 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s">
         <v>81</v>
-      </c>
-      <c r="G3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1655,21 +1655,21 @@
         <v>5000</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1678,24 +1678,24 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
         <v>87</v>
-      </c>
-      <c r="G5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1704,21 +1704,21 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1727,24 +1727,24 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1753,21 +1753,21 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1776,24 +1776,24 @@
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1802,24 +1802,24 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -1828,24 +1828,24 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1854,24 +1854,24 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -1880,24 +1880,24 @@
         <v>14000</v>
       </c>
       <c r="F13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" t="s">
         <v>106</v>
-      </c>
-      <c r="G13" t="s">
-        <v>107</v>
-      </c>
-      <c r="H13" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D14">
         <v>12</v>
@@ -1906,24 +1906,24 @@
         <v>317</v>
       </c>
       <c r="F14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" t="s">
         <v>110</v>
-      </c>
-      <c r="G14" t="s">
-        <v>111</v>
-      </c>
-      <c r="H14" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D15">
         <v>13</v>
@@ -1932,24 +1932,24 @@
         <v>1385</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D16">
         <v>14</v>
@@ -1958,24 +1958,24 @@
         <v>3400</v>
       </c>
       <c r="F16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" t="s">
         <v>117</v>
-      </c>
-      <c r="G16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H16" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D17">
         <v>15</v>
@@ -1984,24 +1984,24 @@
         <v>415</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D18">
         <v>16</v>
@@ -2010,24 +2010,24 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D19">
         <v>17</v>
@@ -2036,24 +2036,24 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D20">
         <v>18</v>
@@ -2062,21 +2062,21 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D21">
         <v>19</v>
@@ -2085,21 +2085,21 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -2108,21 +2108,21 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D23">
         <v>21</v>
@@ -2131,21 +2131,21 @@
         <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D24">
         <v>22</v>
@@ -2154,21 +2154,21 @@
         <v>562.32000000000005</v>
       </c>
       <c r="F24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D25">
         <v>23</v>
@@ -2177,21 +2177,21 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D26">
         <v>24</v>
@@ -2200,21 +2200,21 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D27">
         <v>25</v>
@@ -2223,21 +2223,21 @@
         <v>0.15</v>
       </c>
       <c r="F27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D28">
         <v>26</v>
@@ -2246,21 +2246,21 @@
         <v>0.75</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D29">
         <v>27</v>
@@ -2269,21 +2269,21 @@
         <v>1.5</v>
       </c>
       <c r="F29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D30">
         <v>28</v>
@@ -2292,21 +2292,21 @@
         <v>8961.2676059999994</v>
       </c>
       <c r="F30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D31">
         <v>29</v>
@@ -2315,21 +2315,21 @@
         <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D32">
         <v>30</v>
@@ -2338,21 +2338,21 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D33">
         <v>31</v>
@@ -2361,21 +2361,21 @@
         <v>0.125754527</v>
       </c>
       <c r="F33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D34">
         <v>32</v>
@@ -2384,10 +2384,10 @@
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2399,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36620C0E-6B32-4F3F-9283-5A4BD286D36B}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,134 +2413,134 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" t="s">
         <v>162</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>163</v>
-      </c>
-      <c r="D3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
         <v>62</v>
-      </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2550,44 +2550,40 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA7F6E3-DC99-4262-A736-356D2AE9FB2D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>168</v>
+      <c r="D2" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>